<commit_message>
merge reseq into metagenomics tracker
</commit_message>
<xml_diff>
--- a/2019_2022_resequencing/resequence_combined.xlsx
+++ b/2019_2022_resequencing/resequence_combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brookesienkiewicz/Documents/LabNotebook/2019_2022_resequencing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04E4BD5-0791-9E4A-BA7C-D3C59A2DD338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD6D05B-7561-3141-B564-78D680DFFD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2941" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2952" uniqueCount="557">
   <si>
     <t>Tubelabel_species</t>
   </si>
@@ -1692,6 +1692,21 @@
   </si>
   <si>
     <t>8/19 duplicate extracted in box 32</t>
+  </si>
+  <si>
+    <t>check old extract/enrich for higher concentration</t>
+  </si>
+  <si>
+    <t>new extraction is higher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no info on old extraction but new is high </t>
+  </si>
+  <si>
+    <t>check old extract/enrich for higher concentration (but new one is enough)</t>
+  </si>
+  <si>
+    <t>use old extraction</t>
   </si>
 </sst>
 </file>
@@ -2621,23 +2636,22 @@
   <dimension ref="A1:AI222"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="190" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
+      <selection pane="bottomRight" activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="17" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="14.83203125" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="15" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="11" max="12" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="6" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="9" width="15" customWidth="1"/>
+    <col min="10" max="12" width="10.83203125" customWidth="1"/>
     <col min="13" max="13" width="19.1640625" customWidth="1"/>
     <col min="14" max="30" width="10.83203125" customWidth="1"/>
     <col min="31" max="31" width="19.6640625" bestFit="1" customWidth="1"/>
@@ -2752,190 +2766,199 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
         <v>4.83</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="2">
         <v>2019</v>
       </c>
-      <c r="M2" t="s">
-        <v>70</v>
-      </c>
-      <c r="N2">
+      <c r="M2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" s="2">
         <v>217.9</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="2">
         <v>24.5</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="2">
         <v>2.41</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="AD2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE2" t="s">
+      <c r="AD2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="AI2" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="2">
         <v>2.81</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="2">
         <v>2019</v>
       </c>
-      <c r="M3" t="s">
-        <v>70</v>
-      </c>
-      <c r="N3">
+      <c r="M3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" s="2">
         <v>177.9</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="2">
         <v>29.6</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Y3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z3" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AA3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC3" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="AD3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE3" t="s">
+      <c r="AD3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AF3" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AG3" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AH3" s="2" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="AI3" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <v>17.600000000000001</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="2">
         <v>2019</v>
       </c>
-      <c r="M4" t="s">
-        <v>70</v>
-      </c>
-      <c r="N4">
+      <c r="M4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N4" s="2">
         <v>353.2</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="2">
         <v>9.48</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Y4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="Z4" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AA4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AC4" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="AD4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE4" t="s">
+      <c r="AD4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AF4" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AG4" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AH4" s="2" t="s">
         <v>525</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="5" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3921,60 +3944,63 @@
         <v>525</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="2">
         <v>2019</v>
       </c>
-      <c r="M20" t="s">
-        <v>70</v>
-      </c>
-      <c r="N20">
+      <c r="M20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N20" s="2">
         <v>206.1</v>
       </c>
-      <c r="O20" t="s">
+      <c r="O20" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="2">
         <v>14.3</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Y20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="Z20" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="AA20" t="s">
+      <c r="AA20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC20" t="s">
+      <c r="AC20" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="AD20" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE20" t="s">
+      <c r="AD20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF20" t="s">
+      <c r="AF20" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="AG20" t="s">
+      <c r="AG20" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="AH20" t="s">
+      <c r="AH20" s="2" t="s">
         <v>525</v>
+      </c>
+      <c r="AI20" s="2" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="21" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4033,143 +4059,149 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>0.89</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="2">
         <v>3.67</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="2">
         <v>2019</v>
       </c>
-      <c r="M22" t="s">
-        <v>70</v>
-      </c>
-      <c r="N22">
+      <c r="M22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N22" s="2">
         <v>287.60000000000002</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="2">
         <v>0.78800000000000003</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="Q22" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="R22">
+      <c r="R22" s="2">
         <v>-16.13</v>
       </c>
-      <c r="U22" t="s">
+      <c r="U22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="X22" t="s">
+      <c r="X22" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Y22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="Z22" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AA22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="AC22" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="AD22" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE22" t="s">
+      <c r="AD22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF22" t="s">
+      <c r="AF22" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="AG22" t="s">
+      <c r="AG22" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="AH22" t="s">
+      <c r="AH22" s="2" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="AI22" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="2">
         <v>2019</v>
       </c>
-      <c r="M23" t="s">
-        <v>70</v>
-      </c>
-      <c r="N23">
+      <c r="M23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N23" s="2">
         <v>240.7</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O23" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="2">
         <v>6.52</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Y23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Z23" s="1" t="s">
+      <c r="Z23" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="AA23" t="s">
+      <c r="AA23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC23" t="s">
+      <c r="AC23" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="AD23" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE23" t="s">
+      <c r="AD23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF23" t="s">
+      <c r="AF23" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="AG23" t="s">
+      <c r="AG23" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="AH23" t="s">
+      <c r="AH23" s="2" t="s">
         <v>525</v>
+      </c>
+      <c r="AI23" s="2" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.2">
@@ -5236,6 +5268,9 @@
       <c r="AH41" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="AI41" s="3" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="42" spans="1:35" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
@@ -6548,66 +6583,69 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="65" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="K65" t="s">
+      <c r="K65" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L65">
+      <c r="L65" s="2">
         <v>2019</v>
       </c>
-      <c r="M65" t="s">
-        <v>70</v>
-      </c>
-      <c r="N65">
+      <c r="M65" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N65" s="2">
         <v>219.4</v>
       </c>
-      <c r="O65" t="s">
+      <c r="O65" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="P65">
+      <c r="P65" s="2">
         <v>19</v>
       </c>
-      <c r="Q65" t="s">
+      <c r="Q65" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="R65">
+      <c r="R65" s="2">
         <v>11.1</v>
       </c>
-      <c r="S65" t="s">
+      <c r="S65" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="T65" t="s">
+      <c r="T65" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="U65">
+      <c r="U65" s="2">
         <v>1</v>
       </c>
-      <c r="V65" t="s">
+      <c r="V65" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="W65" t="s">
+      <c r="W65" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="AC65" t="s">
+      <c r="AC65" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="AD65" t="s">
+      <c r="AD65" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AE65" t="s">
+      <c r="AE65" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AG65" t="s">
+      <c r="AG65" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="AH65" t="s">
+      <c r="AH65" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI65" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="66" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>345</v>
       </c>
@@ -6663,7 +6701,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>348</v>
       </c>
@@ -6719,7 +6757,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>393</v>
       </c>
@@ -6775,7 +6813,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>133</v>
       </c>
@@ -6825,7 +6863,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>475</v>
       </c>
@@ -6881,7 +6919,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>96</v>
       </c>
@@ -6922,7 +6960,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>121</v>
       </c>
@@ -6963,7 +7001,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>143</v>
       </c>
@@ -7025,7 +7063,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>132</v>
       </c>
@@ -7066,7 +7104,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>91</v>
       </c>
@@ -7128,7 +7166,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>187</v>
       </c>
@@ -7190,7 +7228,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>136</v>
       </c>
@@ -7231,7 +7269,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>94</v>
       </c>
@@ -7293,7 +7331,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>112</v>
       </c>
@@ -7355,7 +7393,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>117</v>
       </c>
@@ -11191,116 +11229,122 @@
         <v>525</v>
       </c>
     </row>
-    <row r="158" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
+    <row r="158" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D158" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="J158" t="s">
+      <c r="J158" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="K158" t="s">
+      <c r="K158" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="L158">
+      <c r="L158" s="2">
         <v>2019</v>
       </c>
-      <c r="M158" t="s">
-        <v>70</v>
-      </c>
-      <c r="N158">
+      <c r="M158" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N158" s="2">
         <v>204.1</v>
       </c>
-      <c r="O158" t="s">
+      <c r="O158" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="P158">
+      <c r="P158" s="2">
         <v>33.700000000000003</v>
       </c>
-      <c r="Q158" t="s">
+      <c r="Q158" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="Z158" t="s">
+      <c r="Z158" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="AA158" t="s">
+      <c r="AA158" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC158" t="s">
+      <c r="AC158" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="AD158" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE158" t="s">
+      <c r="AD158" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE158" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF158" t="s">
+      <c r="AF158" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="AG158" t="s">
+      <c r="AG158" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="AH158" t="s">
+      <c r="AH158" s="2" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="159" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
+      <c r="AI158" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="159" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="H159" t="s">
+      <c r="H159" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="K159" t="s">
+      <c r="K159" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="L159">
+      <c r="L159" s="2">
         <v>2019</v>
       </c>
-      <c r="M159" t="s">
-        <v>70</v>
-      </c>
-      <c r="N159">
+      <c r="M159" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N159" s="2">
         <v>169.4</v>
       </c>
-      <c r="O159" t="s">
+      <c r="O159" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="P159">
+      <c r="P159" s="2">
         <v>1.1299999999999999</v>
       </c>
-      <c r="Q159" t="s">
+      <c r="Q159" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="Z159" t="s">
+      <c r="Z159" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="AA159" t="s">
+      <c r="AA159" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC159" t="s">
+      <c r="AC159" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AD159" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE159" t="s">
+      <c r="AD159" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE159" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF159" t="s">
+      <c r="AF159" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="AG159" t="s">
+      <c r="AG159" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="AH159" t="s">
+      <c r="AH159" s="2" t="s">
         <v>525</v>
+      </c>
+      <c r="AI159" s="2" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="160" spans="1:35" x14ac:dyDescent="0.2">
@@ -13726,60 +13770,60 @@
         <v>49</v>
       </c>
     </row>
-    <row r="208" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
+    <row r="208" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B208" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="F208" t="s">
+      <c r="F208" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H208" t="s">
+      <c r="H208" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="K208" t="s">
+      <c r="K208" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L208">
+      <c r="L208" s="2">
         <v>2022</v>
       </c>
-      <c r="M208" t="s">
-        <v>70</v>
-      </c>
-      <c r="O208" t="s">
+      <c r="M208" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O208" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="P208">
+      <c r="P208" s="2">
         <v>0.27500000000000002</v>
       </c>
-      <c r="Z208" t="s">
+      <c r="Z208" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="AA208" t="s">
+      <c r="AA208" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC208" t="s">
+      <c r="AC208" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AD208" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE208" t="s">
+      <c r="AD208" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE208" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF208" t="s">
+      <c r="AF208" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AG208" t="s">
+      <c r="AG208" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AH208" t="s">
+      <c r="AH208" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="AI208" t="s">
-        <v>67</v>
+      <c r="AI208" s="2" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="209" spans="1:35" x14ac:dyDescent="0.2">
@@ -13896,63 +13940,63 @@
         <v>67</v>
       </c>
     </row>
-    <row r="211" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A211" t="s">
+    <row r="211" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B211" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="F211" t="s">
+      <c r="F211" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G211" t="s">
+      <c r="G211" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H211" t="s">
+      <c r="H211" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="K211" t="s">
+      <c r="K211" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L211">
+      <c r="L211" s="2">
         <v>2022</v>
       </c>
-      <c r="M211" t="s">
-        <v>70</v>
-      </c>
-      <c r="O211" t="s">
+      <c r="M211" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O211" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="P211">
+      <c r="P211" s="2">
         <v>0.495</v>
       </c>
-      <c r="Z211" t="s">
+      <c r="Z211" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="AA211" t="s">
+      <c r="AA211" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC211" t="s">
+      <c r="AC211" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="AD211" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE211" t="s">
+      <c r="AD211" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE211" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF211" t="s">
+      <c r="AF211" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AG211" t="s">
+      <c r="AG211" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AH211" t="s">
+      <c r="AH211" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="AI211" t="s">
-        <v>67</v>
+      <c r="AI211" s="2" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="212" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -14107,116 +14151,116 @@
         <v>67</v>
       </c>
     </row>
-    <row r="214" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
+    <row r="214" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B214" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="H214" t="s">
+      <c r="H214" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="K214" t="s">
+      <c r="K214" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L214">
+      <c r="L214" s="2">
         <v>2022</v>
       </c>
-      <c r="M214" t="s">
-        <v>70</v>
-      </c>
-      <c r="O214" t="s">
+      <c r="M214" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O214" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="P214">
+      <c r="P214" s="2">
         <v>0.32400000000000001</v>
       </c>
-      <c r="Z214" t="s">
+      <c r="Z214" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="AA214" t="s">
+      <c r="AA214" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC214" t="s">
+      <c r="AC214" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AD214" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE214" t="s">
+      <c r="AD214" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE214" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF214" t="s">
+      <c r="AF214" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="AG214" t="s">
+      <c r="AG214" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AH214" t="s">
+      <c r="AH214" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="AI214" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="215" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A215" t="s">
+      <c r="AI214" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="215" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D215" t="s">
+      <c r="D215" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E215" t="s">
+      <c r="E215" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F215" t="s">
+      <c r="F215" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="G215" t="s">
+      <c r="G215" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H215" t="s">
+      <c r="H215" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="K215" t="s">
+      <c r="K215" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L215">
+      <c r="L215" s="2">
         <v>2019</v>
       </c>
-      <c r="M215" t="s">
-        <v>70</v>
-      </c>
-      <c r="O215" t="s">
+      <c r="M215" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O215" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="P215">
+      <c r="P215" s="2">
         <v>3.19</v>
       </c>
-      <c r="Z215" t="s">
+      <c r="Z215" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="AA215" t="s">
+      <c r="AA215" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC215" t="s">
+      <c r="AC215" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AD215" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE215" t="s">
+      <c r="AD215" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE215" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AG215" t="s">
+      <c r="AG215" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="AH215" t="s">
+      <c r="AH215" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="AI215" t="s">
-        <v>67</v>
+      <c r="AI215" s="2" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="216" spans="1:35" x14ac:dyDescent="0.2">
@@ -14278,54 +14322,57 @@
         <v>67</v>
       </c>
     </row>
-    <row r="217" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A217" t="s">
+    <row r="217" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B217" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="H217" t="s">
+      <c r="H217" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="K217" t="s">
+      <c r="K217" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="L217">
+      <c r="L217" s="2">
         <v>2019</v>
       </c>
-      <c r="M217" t="s">
-        <v>70</v>
-      </c>
-      <c r="O217" t="s">
+      <c r="M217" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O217" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="P217">
+      <c r="P217" s="2">
         <v>0.84099999999999997</v>
       </c>
-      <c r="Z217" t="s">
+      <c r="Z217" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="AA217" t="s">
+      <c r="AA217" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC217" t="s">
+      <c r="AC217" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="AD217" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE217" t="s">
+      <c r="AD217" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE217" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF217" t="s">
+      <c r="AF217" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="AG217" t="s">
+      <c r="AG217" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="AH217" t="s">
+      <c r="AH217" s="2" t="s">
         <v>525</v>
+      </c>
+      <c r="AI217" s="2" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="218" spans="1:35" x14ac:dyDescent="0.2">
@@ -14363,51 +14410,51 @@
         <v>525</v>
       </c>
     </row>
-    <row r="219" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A219" t="s">
+    <row r="219" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H219" t="s">
+      <c r="H219" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K219" t="s">
+      <c r="K219" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="L219">
+      <c r="L219" s="2">
         <v>2022</v>
       </c>
-      <c r="M219" t="s">
-        <v>70</v>
-      </c>
-      <c r="O219" t="s">
+      <c r="M219" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O219" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="P219">
+      <c r="P219" s="2">
         <v>0.105</v>
       </c>
-      <c r="Z219" t="s">
+      <c r="Z219" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="AC219" t="s">
+      <c r="AC219" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AD219" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE219" t="s">
+      <c r="AD219" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE219" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF219" t="s">
+      <c r="AF219" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AG219" t="s">
+      <c r="AG219" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AH219" t="s">
+      <c r="AH219" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="AI219" t="s">
-        <v>67</v>
+      <c r="AI219" s="2" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="220" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>